<commit_message>
Customer and Milestone Page Fixed
</commit_message>
<xml_diff>
--- a/IEC_Invoice_template.xlsx
+++ b/IEC_Invoice_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VIT\Sem4\GeneratePDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callo\OneDrive\Desktop\Office\Invoice-Generator-using-Electron.js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C54FB4-F8D2-4597-8961-0F04876B32F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7729DC-6A46-420F-93BE-4D89DE545227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Invoice 2" sheetId="9" r:id="rId1"/>
+    <sheet name="Invoice" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Invoice 2'!$A$1:$F$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$F$57</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2010-2014 Vertex42 LLC"</definedName>
     <definedName name="vertex42_id" hidden="1">"invoice-template.xlsx"</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>INVOICE</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>SGST</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>IFSC no. - ICIC0000985</t>
@@ -657,7 +654,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -765,6 +762,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
@@ -1140,13 +1141,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1214,13 +1215,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1517,22 +1518,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.09765625" customWidth="1"/>
-    <col min="2" max="2" width="22.69921875" customWidth="1"/>
-    <col min="3" max="3" width="14.09765625" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
     <col min="4" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="15.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1563,7 +1564,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="9"/>
       <c r="E5" s="11" t="s">
@@ -1573,234 +1574,214 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="91"/>
-      <c r="B13" s="91"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="92"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="92"/>
-      <c r="B14" s="92"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="45"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="93"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="40"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="93"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="92"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="92" t="s">
+      <c r="B17" s="93"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="16"/>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="81"/>
+      <c r="C19" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="90"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="84"/>
+    </row>
+    <row r="21" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="92"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="88" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="76" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="82" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="89"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="83"/>
-    </row>
-    <row r="20" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="86"/>
-      <c r="B21" s="85"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="39"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="55"/>
-      <c r="B22" s="87"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="44">
-        <f>C22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="84"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="86"/>
-      <c r="B24" s="85"/>
+    <row r="22" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="87"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="56"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+    </row>
+    <row r="24" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="85"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="90"/>
-      <c r="B25" s="85"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="91"/>
+      <c r="B26" s="86"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="34"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="39"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="1"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="34"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="55"/>
-      <c r="B29" s="56"/>
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="56"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="36">
-        <f>F22-F23-F24</f>
+      <c r="A30" s="56"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="36">
+        <f>F23-F24-F25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="7">
-        <f>IF(D31="",1,D31)*C31</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="14">
-        <v>0.09</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
-      </c>
+      <c r="A32" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="7">
-        <f>F30*C32</f>
+        <f>IF(D32="",1,D32)*C32</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="48"/>
+      <c r="A33" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="49"/>
       <c r="C33" s="14">
         <v>0.09</v>
       </c>
@@ -1809,249 +1790,266 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="7">
-        <f>F30*C33</f>
+        <f>F31*C33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="60" t="s">
+      <c r="A34" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="49"/>
+      <c r="C34" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="7">
+        <f>F31*C34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="23">
+        <f>F33+F34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="25">
+        <f>F31+F35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="63"/>
+      <c r="C37" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="7">
+        <f>F31*C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A38" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="23">
-        <f>F32+F33</f>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="37">
+        <f>F36-F37</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="25">
-        <f>F30+F34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="62"/>
-      <c r="C36" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="7">
-        <f>F30*C36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="37">
-        <f>F35-F36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D38" s="24" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D39" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="31"/>
-    </row>
-    <row r="39" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="D39" s="4"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="27"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="70" t="s">
+      <c r="E39" s="5"/>
+      <c r="F39" s="31"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="D40" s="4"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="32"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="49"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="73"/>
       <c r="E41" s="28"/>
-      <c r="F41" s="33"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="51"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="52"/>
       <c r="E42" s="28"/>
       <c r="F42" s="33"/>
     </row>
-    <row r="43" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="54"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="30"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="54"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="51"/>
+      <c r="C43" s="52"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="33"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A44" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="54"/>
+      <c r="C44" s="55"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="69" t="s">
+      <c r="A45" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="54"/>
-      <c r="E45" s="75" t="s">
+      <c r="B45" s="54"/>
+      <c r="C45" s="55"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="54"/>
+      <c r="C46" s="55"/>
+      <c r="E46" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="75"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
+      <c r="F46" s="76"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="67"/>
-      <c r="C47" s="68"/>
-    </row>
-    <row r="53" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="22" t="s">
+      <c r="A47" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="54"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="68"/>
+      <c r="C48" s="69"/>
+    </row>
+    <row r="54" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E53" s="38" t="s">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="13" t="s">
+      <c r="E54" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="35">
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
   </mergeCells>
-  <conditionalFormatting sqref="A20:A37">
+  <conditionalFormatting sqref="A21:A38">
     <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:B27">
+  <conditionalFormatting sqref="B27:B28">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:F29 F30 C31:F33 F34:F35 C36:F36">
+  <conditionalFormatting sqref="C21:F30 F31 C32:F34 F35:F36 C37:F37">
     <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
+  <conditionalFormatting sqref="F38">
     <cfRule type="expression" dxfId="0" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>